<commit_message>
Fix demo for TGOV1
</commit_message>
<xml_diff>
--- a/demo/TGOV1/ieee39_TGOV1DB.xlsx
+++ b/demo/TGOV1/ieee39_TGOV1DB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/demo/demo/debug/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/demo/demo/TGOV1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A40837-C9FE-2541-B05A-BFE422290253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2884A0B-D8D5-6446-958A-9E92FAAB6B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="Line" sheetId="7" r:id="rId6"/>
     <sheet name="Area" sheetId="8" r:id="rId7"/>
     <sheet name="GENROU" sheetId="9" r:id="rId8"/>
-    <sheet name="TOGV1DB" sheetId="10" r:id="rId9"/>
+    <sheet name="TGOV1DB" sheetId="10" r:id="rId9"/>
     <sheet name="IEEEX1" sheetId="11" r:id="rId10"/>
     <sheet name="IEEEST" sheetId="12" r:id="rId11"/>
     <sheet name="BusFreq" sheetId="13" r:id="rId12"/>
@@ -13509,7 +13509,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>